<commit_message>
Adding Select, Joins, Update Topic
</commit_message>
<xml_diff>
--- a/Practice Sheet.xlsx
+++ b/Practice Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axdit\Desktop\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907F65AA-793D-437A-B4BD-1882009F7A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6A449-8522-4C3F-AB71-C91BF4D58127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6326" yWindow="-18514" windowWidth="21403" windowHeight="17794" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="0" windowWidth="21403" windowHeight="12994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>S. No</t>
   </si>
@@ -91,6 +91,42 @@
   </si>
   <si>
     <t> Invalid Tweets</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/swap-salary/</t>
+  </si>
+  <si>
+    <t>Swap Salary</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/duplicate-emails/</t>
+  </si>
+  <si>
+    <t>Duplicate-Emails</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/employees-earning-more-than-their-managers/description/</t>
+  </si>
+  <si>
+    <t> Employees Earning More Than Their Managers</t>
+  </si>
+  <si>
+    <t>Join</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/not-boring-movies/</t>
+  </si>
+  <si>
+    <t>Not Boring Movies</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/classes-more-than-5-students/description/</t>
+  </si>
+  <si>
+    <t>Classes More Than 5 Students</t>
   </si>
 </sst>
 </file>
@@ -489,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.15234375" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -664,12 +700,24 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45550</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
     </row>
@@ -677,12 +725,24 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45550</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
     </row>
@@ -690,12 +750,24 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45550</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
@@ -703,12 +775,24 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4">
+        <v>45550</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
@@ -716,12 +800,24 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45550</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>

</xml_diff>

<commit_message>
Adding Basic Joins Topic
</commit_message>
<xml_diff>
--- a/Practice Sheet.xlsx
+++ b/Practice Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axdit\Desktop\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6A449-8522-4C3F-AB71-C91BF4D58127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232A595C-4BD7-4A62-96A6-0F9ED5FF1CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="0" windowWidth="21403" windowHeight="12994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>S. No</t>
   </si>
@@ -127,6 +127,36 @@
   </si>
   <si>
     <t>Classes More Than 5 Students</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/replace-employee-id-with-the-unique-identifier/description/</t>
+  </si>
+  <si>
+    <t>Replace Employee ID With The Unique Identifier</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/product-sales-analysis-i/description/</t>
+  </si>
+  <si>
+    <t>Product Sales Analysis I</t>
+  </si>
+  <si>
+    <t>Customer Who Visited but Did Not Make Any Transactions</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/customer-who-visited-but-did-not-make-any-transactions/description/</t>
+  </si>
+  <si>
+    <t>Rising Temperature</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rising-temperature/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/employee-bonus/description/</t>
+  </si>
+  <si>
+    <t>Employee Bonus</t>
   </si>
 </sst>
 </file>
@@ -525,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.15234375" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -825,12 +855,24 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45551</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
     </row>
@@ -838,12 +880,24 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="4">
+        <v>45551</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="2"/>
     </row>
@@ -851,12 +905,24 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="4">
+        <v>45551</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="2"/>
     </row>
@@ -864,12 +930,24 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="4">
+        <v>45551</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
@@ -877,12 +955,24 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="4">
+        <v>45551</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="2"/>
     </row>

</xml_diff>